<commit_message>
Change in option of time dicretisation: user input option removed, now only daily or time disc. based on RF analysis.
Also correction in Ssurf and Eo max computing.
</commit_message>
<xml_diff>
--- a/trunk/MARMITESutilities/POND_EvaporationCorrection.xlsx
+++ b/trunk/MARMITESutilities/POND_EvaporationCorrection.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="19020" windowHeight="12405" activeTab="1"/>
@@ -10,63 +10,69 @@
     <sheet name="averageDIAG" sheetId="4" r:id="rId1"/>
     <sheet name="Computing" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>PX_w</t>
-  </si>
-  <si>
-    <t>PD_w</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>E0</t>
   </si>
   <si>
-    <t>PDratio</t>
-  </si>
-  <si>
-    <t>E0_corr</t>
-  </si>
-  <si>
-    <t>Wfactor</t>
-  </si>
-  <si>
-    <t>PDw</t>
-  </si>
-  <si>
-    <t>PDh</t>
-  </si>
-  <si>
-    <t>Pl</t>
-  </si>
-  <si>
-    <t>Pvol</t>
-  </si>
-  <si>
-    <t>Pxarea</t>
-  </si>
-  <si>
-    <t>Hpx</t>
-  </si>
-  <si>
-    <t>VOLUME</t>
-  </si>
-  <si>
-    <t>FLUXES</t>
-  </si>
-  <si>
-    <t>DIAG correction</t>
+    <t>PD</t>
+  </si>
+  <si>
+    <t>pond</t>
+  </si>
+  <si>
+    <t>ShapeFactor</t>
+  </si>
+  <si>
+    <t>E0_mm</t>
+  </si>
+  <si>
+    <t>PD_w_m</t>
+  </si>
+  <si>
+    <t>PDarea_m2</t>
+  </si>
+  <si>
+    <t>PDw_m</t>
+  </si>
+  <si>
+    <t>PDh_m</t>
+  </si>
+  <si>
+    <t>cell size_m</t>
+  </si>
+  <si>
+    <t>PDarea_ha</t>
+  </si>
+  <si>
+    <t>E0corr_mm</t>
+  </si>
+  <si>
+    <t>E0corr_mm_FORMULA</t>
+  </si>
+  <si>
+    <t>PDvol_m3</t>
+  </si>
+  <si>
+    <t>PD_mm</t>
+  </si>
+  <si>
+    <t>PDvol_m3_ha</t>
+  </si>
+  <si>
+    <t>PD_mm_FORMULA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,13 +80,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -92,13 +130,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -398,601 +443,599 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
-        <f>1/COS(C1)</f>
+        <f t="shared" ref="A1:A45" si="0">1/COS(C1)</f>
         <v>1.0001523280439077</v>
       </c>
       <c r="B1">
         <v>1</v>
       </c>
       <c r="C1">
-        <f>RADIANS(B1)</f>
+        <f t="shared" ref="C1:C45" si="1">RADIANS(B1)</f>
         <v>1.7453292519943295E-2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1">
+        <f>AVERAGE(A1:A45)</f>
+        <v>1.1268477837137569</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>1/COS(C2)</f>
+        <f t="shared" si="0"/>
         <v>1.0006095442988217</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
       <c r="C2">
-        <f>RADIANS(B2)</f>
+        <f t="shared" si="1"/>
         <v>3.4906585039886591E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>1/COS(C3)</f>
+        <f t="shared" si="0"/>
         <v>1.0013723459979209</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3">
-        <f>RADIANS(B3)</f>
+        <f t="shared" si="1"/>
         <v>5.235987755982989E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>1/COS(C4)</f>
+        <f t="shared" si="0"/>
         <v>1.0024418980811722</v>
       </c>
       <c r="B4">
         <v>4</v>
       </c>
       <c r="C4">
-        <f>RADIANS(B4)</f>
+        <f t="shared" si="1"/>
         <v>6.9813170079773182E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>1/COS(C5)</f>
+        <f t="shared" si="0"/>
         <v>1.0038198375433474</v>
       </c>
       <c r="B5">
         <v>5</v>
       </c>
       <c r="C5">
-        <f>RADIANS(B5)</f>
+        <f t="shared" si="1"/>
         <v>8.7266462599716474E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>1/COS(C6)</f>
+        <f t="shared" si="0"/>
         <v>1.0055082795635164</v>
       </c>
       <c r="B6">
         <v>6</v>
       </c>
       <c r="C6">
-        <f>RADIANS(B6)</f>
+        <f t="shared" si="1"/>
         <v>0.10471975511965978</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>1/COS(C7)</f>
+        <f t="shared" si="0"/>
         <v>1.0075098254588484</v>
       </c>
       <c r="B7">
         <v>7</v>
       </c>
       <c r="C7">
-        <f>RADIANS(B7)</f>
+        <f t="shared" si="1"/>
         <v>0.12217304763960307</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>1/COS(C8)</f>
+        <f t="shared" si="0"/>
         <v>1.0098275725186181</v>
       </c>
       <c r="B8">
         <v>8</v>
       </c>
       <c r="C8">
-        <f>RADIANS(B8)</f>
+        <f t="shared" si="1"/>
         <v>0.13962634015954636</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>1/COS(C9)</f>
+        <f t="shared" si="0"/>
         <v>1.0124651257880029</v>
       </c>
       <c r="B9">
         <v>9</v>
       </c>
       <c r="C9">
-        <f>RADIANS(B9)</f>
+        <f t="shared" si="1"/>
         <v>0.15707963267948966</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f>1/COS(C10)</f>
+        <f t="shared" si="0"/>
         <v>1.0154266118857451</v>
       </c>
       <c r="B10">
         <v>10</v>
       </c>
       <c r="C10">
-        <f>RADIANS(B10)</f>
+        <f t="shared" si="1"/>
         <v>0.17453292519943295</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>1/COS(C11)</f>
+        <f t="shared" si="0"/>
         <v>1.0187166949552142</v>
       </c>
       <c r="B11">
         <v>11</v>
       </c>
       <c r="C11">
-        <f>RADIANS(B11)</f>
+        <f t="shared" si="1"/>
         <v>0.19198621771937624</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>1/COS(C12)</f>
+        <f t="shared" si="0"/>
         <v>1.0223405948650293</v>
       </c>
       <c r="B12">
         <v>12</v>
       </c>
       <c r="C12">
-        <f>RADIANS(B12)</f>
+        <f t="shared" si="1"/>
         <v>0.20943951023931956</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>1/COS(C13)</f>
+        <f t="shared" si="0"/>
         <v>1.0263041077933917</v>
       </c>
       <c r="B13">
         <v>13</v>
       </c>
       <c r="C13">
-        <f>RADIANS(B13)</f>
+        <f t="shared" si="1"/>
         <v>0.22689280275926285</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>1/COS(C14)</f>
+        <f t="shared" si="0"/>
         <v>1.0306136293498982</v>
       </c>
       <c r="B14">
         <v>14</v>
       </c>
       <c r="C14">
-        <f>RADIANS(B14)</f>
+        <f t="shared" si="1"/>
         <v>0.24434609527920614</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f>1/COS(C15)</f>
+        <f t="shared" si="0"/>
         <v>1.035276180410083</v>
       </c>
       <c r="B15">
         <v>15</v>
       </c>
       <c r="C15">
-        <f>RADIANS(B15)</f>
+        <f t="shared" si="1"/>
         <v>0.26179938779914941</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>1/COS(C16)</f>
+        <f t="shared" si="0"/>
         <v>1.040299435861602</v>
       </c>
       <c r="B16">
         <v>16</v>
       </c>
       <c r="C16">
-        <f>RADIANS(B16)</f>
+        <f t="shared" si="1"/>
         <v>0.27925268031909273</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f>1/COS(C17)</f>
+        <f t="shared" si="0"/>
         <v>1.045691756487148</v>
       </c>
       <c r="B17">
         <v>17</v>
       </c>
       <c r="C17">
-        <f>RADIANS(B17)</f>
+        <f t="shared" si="1"/>
         <v>0.29670597283903605</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>1/COS(C18)</f>
+        <f t="shared" si="0"/>
         <v>1.0514622242382672</v>
       </c>
       <c r="B18">
         <v>18</v>
       </c>
       <c r="C18">
-        <f>RADIANS(B18)</f>
+        <f t="shared" si="1"/>
         <v>0.31415926535897931</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>1/COS(C19)</f>
+        <f t="shared" si="0"/>
         <v>1.0576206811866706</v>
       </c>
       <c r="B19">
         <v>19</v>
       </c>
       <c r="C19">
-        <f>RADIANS(B19)</f>
+        <f t="shared" si="1"/>
         <v>0.33161255787892263</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>1/COS(C20)</f>
+        <f t="shared" si="0"/>
         <v>1.0641777724759121</v>
       </c>
       <c r="B20">
         <v>20</v>
       </c>
       <c r="C20">
-        <f>RADIANS(B20)</f>
+        <f t="shared" si="1"/>
         <v>0.3490658503988659</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f>1/COS(C21)</f>
+        <f t="shared" si="0"/>
         <v>1.071144993637029</v>
       </c>
       <c r="B21">
         <v>21</v>
       </c>
       <c r="C21">
-        <f>RADIANS(B21)</f>
+        <f t="shared" si="1"/>
         <v>0.36651914291880922</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>1/COS(C22)</f>
+        <f t="shared" si="0"/>
         <v>1.0785347426775833</v>
       </c>
       <c r="B22">
         <v>22</v>
       </c>
       <c r="C22">
-        <f>RADIANS(B22)</f>
+        <f t="shared" si="1"/>
         <v>0.38397243543875248</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>1/COS(C23)</f>
+        <f t="shared" si="0"/>
         <v>1.0863603774052961</v>
       </c>
       <c r="B23">
         <v>23</v>
       </c>
       <c r="C23">
-        <f>RADIANS(B23)</f>
+        <f t="shared" si="1"/>
         <v>0.4014257279586958</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>1/COS(C24)</f>
+        <f t="shared" si="0"/>
         <v>1.0946362785060468</v>
       </c>
       <c r="B24">
         <v>24</v>
       </c>
       <c r="C24">
-        <f>RADIANS(B24)</f>
+        <f t="shared" si="1"/>
         <v>0.41887902047863912</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f>1/COS(C25)</f>
+        <f t="shared" si="0"/>
         <v>1.1033779189624917</v>
       </c>
       <c r="B25">
         <v>25</v>
       </c>
       <c r="C25">
-        <f>RADIANS(B25)</f>
+        <f t="shared" si="1"/>
         <v>0.43633231299858238</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f>1/COS(C26)</f>
+        <f t="shared" si="0"/>
         <v>1.1126019404751888</v>
       </c>
       <c r="B26">
         <v>26</v>
       </c>
       <c r="C26">
-        <f>RADIANS(B26)</f>
+        <f t="shared" si="1"/>
         <v>0.4537856055185257</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>1/COS(C27)</f>
+        <f t="shared" si="0"/>
         <v>1.1223262376343608</v>
       </c>
       <c r="B27">
         <v>27</v>
       </c>
       <c r="C27">
-        <f>RADIANS(B27)</f>
+        <f t="shared" si="1"/>
         <v>0.47123889803846897</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f>1/COS(C28)</f>
+        <f t="shared" si="0"/>
         <v>1.132570050689039</v>
       </c>
       <c r="B28">
         <v>28</v>
       </c>
       <c r="C28">
-        <f>RADIANS(B28)</f>
+        <f t="shared" si="1"/>
         <v>0.48869219055841229</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f>1/COS(C29)</f>
+        <f t="shared" si="0"/>
         <v>1.1433540678733201</v>
       </c>
       <c r="B29">
         <v>29</v>
       </c>
       <c r="C29">
-        <f>RADIANS(B29)</f>
+        <f t="shared" si="1"/>
         <v>0.50614548307835561</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f>1/COS(C30)</f>
+        <f t="shared" si="0"/>
         <v>1.1547005383792515</v>
       </c>
       <c r="B30">
         <v>30</v>
       </c>
       <c r="C30">
-        <f>RADIANS(B30)</f>
+        <f t="shared" si="1"/>
         <v>0.52359877559829882</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f>1/COS(C31)</f>
+        <f t="shared" si="0"/>
         <v>1.1666333972153304</v>
       </c>
       <c r="B31">
         <v>31</v>
       </c>
       <c r="C31">
-        <f>RADIANS(B31)</f>
+        <f t="shared" si="1"/>
         <v>0.54105206811824214</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f>1/COS(C32)</f>
+        <f t="shared" si="0"/>
         <v>1.1791784033620965</v>
       </c>
       <c r="B32">
         <v>32</v>
       </c>
       <c r="C32">
-        <f>RADIANS(B32)</f>
+        <f t="shared" si="1"/>
         <v>0.55850536063818546</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f>1/COS(C33)</f>
+        <f t="shared" si="0"/>
         <v>1.1923632928359473</v>
       </c>
       <c r="B33">
         <v>33</v>
       </c>
       <c r="C33">
-        <f>RADIANS(B33)</f>
+        <f t="shared" si="1"/>
         <v>0.57595865315812877</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f>1/COS(C34)</f>
+        <f t="shared" si="0"/>
         <v>1.2062179485039055</v>
       </c>
       <c r="B34">
         <v>34</v>
       </c>
       <c r="C34">
-        <f>RADIANS(B34)</f>
+        <f t="shared" si="1"/>
         <v>0.59341194567807209</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f>1/COS(C35)</f>
+        <f t="shared" si="0"/>
         <v>1.2207745887614561</v>
       </c>
       <c r="B35">
         <v>35</v>
       </c>
       <c r="C35">
-        <f>RADIANS(B35)</f>
+        <f t="shared" si="1"/>
         <v>0.6108652381980153</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f>1/COS(C36)</f>
+        <f t="shared" si="0"/>
         <v>1.2360679774997896</v>
       </c>
       <c r="B36">
         <v>36</v>
       </c>
       <c r="C36">
-        <f>RADIANS(B36)</f>
+        <f t="shared" si="1"/>
         <v>0.62831853071795862</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f>1/COS(C37)</f>
+        <f t="shared" si="0"/>
         <v>1.2521356581562257</v>
       </c>
       <c r="B37">
         <v>37</v>
       </c>
       <c r="C37">
-        <f>RADIANS(B37)</f>
+        <f t="shared" si="1"/>
         <v>0.64577182323790194</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f>1/COS(C38)</f>
+        <f t="shared" si="0"/>
         <v>1.2690182150725788</v>
       </c>
       <c r="B38">
         <v>38</v>
       </c>
       <c r="C38">
-        <f>RADIANS(B38)</f>
+        <f t="shared" si="1"/>
         <v>0.66322511575784526</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f>1/COS(C39)</f>
+        <f t="shared" si="0"/>
         <v>1.2867595658931672</v>
       </c>
       <c r="B39">
         <v>39</v>
       </c>
       <c r="C39">
-        <f>RADIANS(B39)</f>
+        <f t="shared" si="1"/>
         <v>0.68067840827778847</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f>1/COS(C40)</f>
+        <f t="shared" si="0"/>
         <v>1.3054072893322786</v>
       </c>
       <c r="B40">
         <v>40</v>
       </c>
       <c r="C40">
-        <f>RADIANS(B40)</f>
+        <f t="shared" si="1"/>
         <v>0.69813170079773179</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f>1/COS(C41)</f>
+        <f t="shared" si="0"/>
         <v>1.3250129933488113</v>
       </c>
       <c r="B41">
         <v>41</v>
       </c>
       <c r="C41">
-        <f>RADIANS(B41)</f>
+        <f t="shared" si="1"/>
         <v>0.71558499331767511</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f>1/COS(C42)</f>
+        <f t="shared" si="0"/>
         <v>1.3456327296063761</v>
       </c>
       <c r="B42">
         <v>42</v>
       </c>
       <c r="C42">
-        <f>RADIANS(B42)</f>
+        <f t="shared" si="1"/>
         <v>0.73303828583761843</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f>1/COS(C43)</f>
+        <f t="shared" si="0"/>
         <v>1.3673274610985953</v>
       </c>
       <c r="B43">
         <v>43</v>
       </c>
       <c r="C43">
-        <f>RADIANS(B43)</f>
+        <f t="shared" si="1"/>
         <v>0.75049157835756175</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f>1/COS(C44)</f>
+        <f t="shared" si="0"/>
         <v>1.3901635910166787</v>
       </c>
       <c r="B44">
         <v>44</v>
       </c>
       <c r="C44">
-        <f>RADIANS(B44)</f>
+        <f t="shared" si="1"/>
         <v>0.76794487087750496</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f>1/COS(C45)</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730949</v>
       </c>
       <c r="B45">
         <v>45</v>
       </c>
       <c r="C45">
-        <f>RADIANS(B45)</f>
+        <f t="shared" si="1"/>
         <v>0.78539816339744828</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <f>AVERAGE(A1:A45)</f>
-        <v>1.1268477837137569</v>
       </c>
     </row>
   </sheetData>
@@ -1002,63 +1045,124 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="3">
+        <v>100</v>
+      </c>
+      <c r="C2" s="3">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2">
+        <f>C2*$K$3*B2</f>
+        <v>112.6847783713757</v>
+      </c>
+      <c r="E2">
+        <f>D2/100^2</f>
+        <v>1.126847783713757E-2</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2">
+        <f>E2*F2</f>
+        <v>3.3805433511412714E-2</v>
+      </c>
+      <c r="H2" s="2">
+        <f>B2*C2*$K$3*F2/100^2</f>
+        <v>3.3805433511412707E-2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="3">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <f>C3*$K$3*B3</f>
+        <v>11.268477837137569</v>
+      </c>
+      <c r="E3">
+        <f>D3/100^2</f>
+        <v>1.1268477837137569E-3</v>
+      </c>
+      <c r="F3">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2">
-        <v>100</v>
-      </c>
-      <c r="C2">
+      <c r="G3" s="2">
+        <f>E3*F3</f>
+        <v>3.3805433511412708E-3</v>
+      </c>
+      <c r="H3" s="2">
+        <f>B3*C3*$K$3*F3/100^2</f>
+        <v>3.3805433511412708E-3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <f>averageDIAG!E1</f>
+        <v>1.1268477837137569</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="G2">
-        <f>C2*E2/B2</f>
-        <v>1.1200000000000002E-2</v>
-      </c>
-      <c r="H2">
-        <f>D2*G2</f>
-        <v>3.3600000000000005E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -1067,61 +1171,97 @@
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>100</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <f>C8*D8*B8*$K$3</f>
+        <v>225.3695567427514</v>
+      </c>
+      <c r="F8">
+        <f>E8*B8^2/100^2</f>
+        <v>225.3695567427514</v>
+      </c>
+      <c r="G8" s="2">
+        <f>F8/10</f>
+        <v>22.536955674275141</v>
+      </c>
+      <c r="H8" s="2">
+        <f>C8*D8*B8*$K$3*B8^2/100^2/10</f>
+        <v>22.536955674275141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
         <v>10</v>
       </c>
-      <c r="G7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
+      <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="C8">
+      <c r="D9" s="3">
         <v>2</v>
       </c>
-      <c r="D8">
-        <v>112</v>
-      </c>
-      <c r="E8">
-        <f>B8*C8*D8</f>
-        <v>224</v>
-      </c>
-      <c r="F8">
-        <f>100*100</f>
-        <v>10000</v>
-      </c>
-      <c r="G8">
-        <f>E8/F8</f>
-        <v>2.24E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="C9">
+      <c r="E9">
+        <f t="shared" ref="E9:E10" si="0">C9*D9*B9*$K$3</f>
+        <v>22.536955674275138</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9:F10" si="1">E9*B9^2/100^2</f>
+        <v>0.22536955674275136</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" ref="G9:G10" si="2">F9/10</f>
+        <v>2.2536955674275137E-2</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" ref="H9:H10" si="3">C9*D9*B9*$K$3*B9^2/100^2/10</f>
+        <v>2.2536955674275137E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
+        <v>50</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
         <v>2</v>
       </c>
-      <c r="D9">
-        <v>100</v>
-      </c>
-      <c r="E9">
-        <f>B9*C9*D9</f>
-        <v>224.00000000000003</v>
-      </c>
-      <c r="G9">
-        <f>C9*B9/D9</f>
-        <v>2.2400000000000003E-2</v>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>112.6847783713757</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>28.171194592843925</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="2"/>
+        <v>2.8171194592843927</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="3"/>
+        <v>2.8171194592843927</v>
       </c>
     </row>
   </sheetData>

</xml_diff>